<commit_message>
check in from RTC
</commit_message>
<xml_diff>
--- a/documentation/MHIDBSchema2.xlsx
+++ b/documentation/MHIDBSchema2.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mczapanskiy\Documents\GitHub\WERC-SC\documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20085" windowHeight="9375" tabRatio="500" activeTab="1"/>
   </bookViews>
@@ -18,7 +13,7 @@
     <sheet name="ACC" sheetId="4" r:id="rId4"/>
     <sheet name="Lists" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="146">
   <si>
     <t>Field</t>
   </si>
@@ -375,9 +370,6 @@
     <t>DiveFlag</t>
   </si>
   <si>
-    <t>Not currently implemented, could be useful in the future if we differentiate U-, V-, W-, and J-dives.</t>
-  </si>
-  <si>
     <t>Dive</t>
   </si>
   <si>
@@ -460,6 +452,15 @@
   </si>
   <si>
     <t>PK, not null</t>
+  </si>
+  <si>
+    <t>Dive quality - result from the QAQC process</t>
+  </si>
+  <si>
+    <t>PlungeErr</t>
+  </si>
+  <si>
+    <t>SplitErr</t>
   </si>
 </sst>
 </file>
@@ -587,7 +588,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -610,6 +611,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -622,7 +627,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1013,7 +1017,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1027,7 +1031,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1039,7 +1043,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1051,25 +1055,25 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="C6" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1083,7 +1087,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
@@ -1095,7 +1099,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
@@ -1107,7 +1111,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
@@ -1119,7 +1123,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
@@ -1131,7 +1135,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
@@ -1143,7 +1147,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1152,59 +1156,59 @@
       <c r="C13" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="17" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="15"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="15"/>
+      <c r="D16" s="17"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="15"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="15"/>
+      <c r="D18" s="17"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
@@ -1215,7 +1219,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="16" t="s">
         <v>94</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1229,7 +1233,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="7" t="s">
         <v>23</v>
       </c>
@@ -1238,7 +1242,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="7" t="s">
         <v>24</v>
       </c>
@@ -1247,7 +1251,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="7" t="s">
         <v>25</v>
       </c>
@@ -1256,7 +1260,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="7" t="s">
         <v>26</v>
       </c>
@@ -1265,7 +1269,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="7" t="s">
         <v>27</v>
       </c>
@@ -1274,7 +1278,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="7" t="s">
         <v>28</v>
       </c>
@@ -1283,7 +1287,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="7" t="s">
         <v>29</v>
       </c>
@@ -1292,7 +1296,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="7" t="s">
         <v>30</v>
       </c>
@@ -1301,7 +1305,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="7" t="s">
         <v>31</v>
       </c>
@@ -1310,7 +1314,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="7" t="s">
         <v>32</v>
       </c>
@@ -1319,7 +1323,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="7" t="s">
         <v>33</v>
       </c>
@@ -1328,7 +1332,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="7" t="s">
         <v>34</v>
       </c>
@@ -1337,7 +1341,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="7" t="s">
         <v>35</v>
       </c>
@@ -1346,7 +1350,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="7" t="s">
         <v>36</v>
       </c>
@@ -1355,7 +1359,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="7" t="s">
         <v>37</v>
       </c>
@@ -1364,7 +1368,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="7" t="s">
         <v>38</v>
       </c>
@@ -1373,7 +1377,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="7" t="s">
         <v>39</v>
       </c>
@@ -1382,7 +1386,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="16"/>
       <c r="B38" s="7" t="s">
         <v>40</v>
       </c>
@@ -1391,7 +1395,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="16"/>
       <c r="B39" s="7" t="s">
         <v>41</v>
       </c>
@@ -1400,7 +1404,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="16"/>
       <c r="B40" s="7" t="s">
         <v>42</v>
       </c>
@@ -1409,7 +1413,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="16"/>
       <c r="B41" s="7" t="s">
         <v>43</v>
       </c>
@@ -1418,7 +1422,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="7" t="s">
         <v>44</v>
       </c>
@@ -1427,7 +1431,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="7" t="s">
         <v>45</v>
       </c>
@@ -1436,7 +1440,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="7" t="s">
         <v>46</v>
       </c>
@@ -1445,7 +1449,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
+      <c r="A45" s="16"/>
       <c r="B45" s="7" t="s">
         <v>47</v>
       </c>
@@ -1454,7 +1458,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="7" t="s">
         <v>48</v>
       </c>
@@ -1463,7 +1467,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="16"/>
       <c r="B47" s="7" t="s">
         <v>49</v>
       </c>
@@ -1472,7 +1476,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="A48" s="16"/>
       <c r="B48" s="7" t="s">
         <v>50</v>
       </c>
@@ -1481,7 +1485,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="16"/>
       <c r="B49" s="7" t="s">
         <v>51</v>
       </c>
@@ -1490,7 +1494,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="7" t="s">
         <v>52</v>
       </c>
@@ -1499,7 +1503,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="7" t="s">
         <v>53</v>
       </c>
@@ -1508,7 +1512,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="7" t="s">
         <v>54</v>
       </c>
@@ -1517,7 +1521,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="7" t="s">
         <v>55</v>
       </c>
@@ -1526,7 +1530,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="7" t="s">
         <v>56</v>
       </c>
@@ -1535,7 +1539,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="7" t="s">
         <v>57</v>
       </c>
@@ -1544,7 +1548,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
+      <c r="A56" s="16"/>
       <c r="B56" s="7" t="s">
         <v>58</v>
       </c>
@@ -1553,7 +1557,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="7" t="s">
         <v>59</v>
       </c>
@@ -1562,7 +1566,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
+      <c r="A58" s="16"/>
       <c r="B58" s="7" t="s">
         <v>60</v>
       </c>
@@ -1571,7 +1575,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="16"/>
       <c r="B59" s="7" t="s">
         <v>61</v>
       </c>
@@ -1580,7 +1584,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="16"/>
       <c r="B60" s="7" t="s">
         <v>62</v>
       </c>
@@ -1589,7 +1593,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
+      <c r="A61" s="16"/>
       <c r="B61" s="7" t="s">
         <v>63</v>
       </c>
@@ -1598,7 +1602,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="16"/>
       <c r="B62" s="7" t="s">
         <v>64</v>
       </c>
@@ -1607,7 +1611,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+      <c r="A63" s="16"/>
       <c r="B63" s="7" t="s">
         <v>65</v>
       </c>
@@ -1616,7 +1620,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="16"/>
       <c r="B64" s="7" t="s">
         <v>66</v>
       </c>
@@ -1625,7 +1629,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
+      <c r="A65" s="16"/>
       <c r="B65" s="7" t="s">
         <v>67</v>
       </c>
@@ -1634,7 +1638,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
+      <c r="A66" s="16"/>
       <c r="B66" s="7" t="s">
         <v>68</v>
       </c>
@@ -1643,7 +1647,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
+      <c r="A67" s="16"/>
       <c r="B67" s="7" t="s">
         <v>69</v>
       </c>
@@ -1652,7 +1656,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="16"/>
       <c r="B68" s="7" t="s">
         <v>70</v>
       </c>
@@ -1661,7 +1665,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
+      <c r="A69" s="16"/>
       <c r="B69" s="7" t="s">
         <v>71</v>
       </c>
@@ -1670,7 +1674,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="7" t="s">
         <v>72</v>
       </c>
@@ -1679,7 +1683,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
+      <c r="A71" s="16"/>
       <c r="B71" s="7" t="s">
         <v>73</v>
       </c>
@@ -1688,7 +1692,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
+      <c r="A72" s="16"/>
       <c r="B72" s="7" t="s">
         <v>74</v>
       </c>
@@ -1697,7 +1701,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
+      <c r="A73" s="16"/>
       <c r="B73" s="7" t="s">
         <v>75</v>
       </c>
@@ -1706,7 +1710,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
+      <c r="A74" s="16"/>
       <c r="B74" s="7" t="s">
         <v>76</v>
       </c>
@@ -1715,7 +1719,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="16"/>
       <c r="B75" s="7" t="s">
         <v>77</v>
       </c>
@@ -1724,7 +1728,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
+      <c r="A76" s="16"/>
       <c r="B76" s="7" t="s">
         <v>78</v>
       </c>
@@ -1733,7 +1737,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
+      <c r="A77" s="16"/>
       <c r="B77" s="7" t="s">
         <v>79</v>
       </c>
@@ -1742,7 +1746,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="14"/>
+      <c r="A78" s="16"/>
       <c r="B78" s="7" t="s">
         <v>80</v>
       </c>
@@ -1751,7 +1755,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
+      <c r="A79" s="16"/>
       <c r="B79" s="7" t="s">
         <v>81</v>
       </c>
@@ -1760,7 +1764,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
+      <c r="A80" s="16"/>
       <c r="B80" s="7" t="s">
         <v>82</v>
       </c>
@@ -1769,7 +1773,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
+      <c r="A81" s="16"/>
       <c r="B81" s="7" t="s">
         <v>83</v>
       </c>
@@ -1778,7 +1782,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
+      <c r="A82" s="16"/>
       <c r="B82" s="7" t="s">
         <v>84</v>
       </c>
@@ -1787,7 +1791,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
+      <c r="A83" s="16"/>
       <c r="B83" s="7" t="s">
         <v>85</v>
       </c>
@@ -1796,7 +1800,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
+      <c r="A84" s="16"/>
       <c r="B84" s="7" t="s">
         <v>86</v>
       </c>
@@ -1805,7 +1809,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
+      <c r="A85" s="16"/>
       <c r="B85" s="7" t="s">
         <v>87</v>
       </c>
@@ -1814,7 +1818,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
+      <c r="A86" s="16"/>
       <c r="B86" s="7" t="s">
         <v>88</v>
       </c>
@@ -1823,7 +1827,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
+      <c r="A87" s="16"/>
       <c r="B87" s="7" t="s">
         <v>89</v>
       </c>
@@ -1832,7 +1836,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="14"/>
+      <c r="A88" s="16"/>
       <c r="B88" s="7" t="s">
         <v>90</v>
       </c>
@@ -1841,7 +1845,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
+      <c r="A89" s="16"/>
       <c r="B89" s="7" t="s">
         <v>91</v>
       </c>
@@ -1850,7 +1854,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="14"/>
+      <c r="A90" s="16"/>
       <c r="B90" s="7" t="s">
         <v>92</v>
       </c>
@@ -1859,7 +1863,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="14"/>
+      <c r="A91" s="16"/>
       <c r="B91" s="7" t="s">
         <v>93</v>
       </c>
@@ -1887,10 +1891,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1914,8 +1918,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>116</v>
+      <c r="A2" s="18" t="s">
+        <v>115</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>109</v>
@@ -1924,25 +1928,25 @@
         <v>97</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="18" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="15" t="s">
         <v>110</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>97</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>95</v>
@@ -1952,9 +1956,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>95</v>
@@ -1964,7 +1968,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="5" t="s">
         <v>111</v>
       </c>
@@ -1972,11 +1976,11 @@
         <v>96</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="5" t="s">
         <v>112</v>
       </c>
@@ -1984,11 +1988,11 @@
         <v>96</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="5" t="s">
         <v>113</v>
       </c>
@@ -1996,686 +2000,704 @@
         <v>97</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="7" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="7" t="s">
+      <c r="C14" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="7" t="s">
+      <c r="C19" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="7" t="s">
+      <c r="C20" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="7" t="s">
+      <c r="C21" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="7" t="s">
+      <c r="C22" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="7" t="s">
+      <c r="C23" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="7" t="s">
+      <c r="C24" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="7" t="s">
+      <c r="C25" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="7" t="s">
+      <c r="C26" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="B27" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="7" t="s">
+      <c r="C27" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="7" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
+      <c r="B31" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
+      <c r="B32" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="7" t="s">
+      <c r="C32" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="B33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="7" t="s">
+      <c r="C33" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
+      <c r="B34" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="7" t="s">
+      <c r="C34" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="16"/>
+      <c r="B35" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="7" t="s">
+      <c r="C35" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="16"/>
+      <c r="B36" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="7" t="s">
+      <c r="C36" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="16"/>
+      <c r="B37" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="7" t="s">
+      <c r="C37" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="16"/>
+      <c r="B38" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="7" t="s">
+      <c r="C38" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="16"/>
+      <c r="B39" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="7" t="s">
+      <c r="C39" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
+      <c r="B40" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="7" t="s">
+      <c r="C40" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="16"/>
+      <c r="B41" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="7" t="s">
+      <c r="C41" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="16"/>
+      <c r="B42" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="7" t="s">
+      <c r="C42" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="16"/>
+      <c r="B43" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="7" t="s">
+      <c r="C43" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="16"/>
+      <c r="B44" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="7" t="s">
+      <c r="C44" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="16"/>
+      <c r="B45" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="7" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="16"/>
+      <c r="B46" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="7" t="s">
+      <c r="C46" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="16"/>
+      <c r="B47" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="7" t="s">
+      <c r="C47" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="16"/>
+      <c r="B48" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="7" t="s">
+      <c r="C48" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="16"/>
+      <c r="B49" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="7" t="s">
+      <c r="C49" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
+      <c r="B50" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="7" t="s">
+      <c r="C50" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="16"/>
+      <c r="B51" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="7" t="s">
+      <c r="C51" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="16"/>
+      <c r="B52" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="7" t="s">
+      <c r="C52" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="16"/>
+      <c r="B53" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="7" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="16"/>
+      <c r="B54" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="7" t="s">
+      <c r="C54" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="16"/>
+      <c r="B55" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="7" t="s">
+      <c r="C55" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="16"/>
+      <c r="B56" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
-      <c r="B55" s="7" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="16"/>
+      <c r="B57" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
-      <c r="B56" s="7" t="s">
+      <c r="C57" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="16"/>
+      <c r="B58" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
-      <c r="B57" s="7" t="s">
+      <c r="C58" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="16"/>
+      <c r="B59" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="7" t="s">
+      <c r="C59" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="16"/>
+      <c r="B60" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="7" t="s">
+      <c r="C60" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="16"/>
+      <c r="B61" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C61" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="7" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="16"/>
+      <c r="B62" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="7" t="s">
+      <c r="C62" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="16"/>
+      <c r="B63" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
-      <c r="B62" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
-      <c r="B63" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="16"/>
       <c r="B64" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
+      <c r="A65" s="16"/>
       <c r="B65" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="16"/>
+      <c r="B66" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="16"/>
+      <c r="B67" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="7" t="s">
+      <c r="C67" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="16"/>
+      <c r="B68" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
-      <c r="B67" s="7" t="s">
+      <c r="C68" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="16"/>
+      <c r="B69" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C67" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
-      <c r="B68" s="7" t="s">
+      <c r="C69" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="16"/>
+      <c r="B70" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="7" t="s">
+      <c r="C70" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="16"/>
+      <c r="B71" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
-      <c r="B70" s="7" t="s">
+      <c r="C71" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="16"/>
+      <c r="B72" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
-      <c r="B71" s="7" t="s">
+      <c r="C72" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="16"/>
+      <c r="B73" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C71" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
-      <c r="B72" s="7" t="s">
+      <c r="C73" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="16"/>
+      <c r="B74" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C74" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="7" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="16"/>
+      <c r="B75" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C75" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
-      <c r="B74" s="7" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="16"/>
+      <c r="B76" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
-      <c r="B75" s="7" t="s">
+      <c r="C76" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="16"/>
+      <c r="B77" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C75" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
-      <c r="B76" s="7" t="s">
+      <c r="C77" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="16"/>
+      <c r="B78" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C76" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
-      <c r="B77" s="7" t="s">
+      <c r="C78" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="16"/>
+      <c r="B79" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="14"/>
-      <c r="B78" s="7" t="s">
+      <c r="C79" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="16"/>
+      <c r="B80" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
-      <c r="B79" s="7" t="s">
+      <c r="C80" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="16"/>
+      <c r="B81" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
-      <c r="B80" s="7" t="s">
+      <c r="C81" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="16"/>
+      <c r="B82" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C80" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
-      <c r="B81" s="7" t="s">
+      <c r="C82" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="16"/>
+      <c r="B83" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C81" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
-      <c r="B82" s="7" t="s">
+      <c r="C83" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="16"/>
+      <c r="B84" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C84" s="4" t="s">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A11:A82"/>
+    <mergeCell ref="A13:A84"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2728,21 +2750,21 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="C2" s="4" t="s">
         <v>97</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
@@ -2750,11 +2772,11 @@
         <v>95</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="5" t="s">
         <v>111</v>
       </c>
@@ -2762,97 +2784,97 @@
         <v>96</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="5" t="s">
+      <c r="C8" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2864,7 +2886,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="16" t="s">
         <v>94</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2878,7 +2900,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="7" t="s">
         <v>23</v>
       </c>
@@ -2887,7 +2909,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
@@ -2896,7 +2918,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
@@ -2905,7 +2927,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
@@ -2914,7 +2936,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="7" t="s">
         <v>27</v>
       </c>
@@ -2923,7 +2945,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="7" t="s">
         <v>28</v>
       </c>
@@ -2932,7 +2954,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="7" t="s">
         <v>29</v>
       </c>
@@ -2941,7 +2963,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="7" t="s">
         <v>30</v>
       </c>
@@ -2950,7 +2972,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="7" t="s">
         <v>31</v>
       </c>
@@ -2959,7 +2981,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="7" t="s">
         <v>32</v>
       </c>
@@ -2968,7 +2990,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="7" t="s">
         <v>33</v>
       </c>
@@ -2977,7 +2999,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="7" t="s">
         <v>34</v>
       </c>
@@ -2986,7 +3008,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="7" t="s">
         <v>35</v>
       </c>
@@ -2995,7 +3017,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="7" t="s">
         <v>36</v>
       </c>
@@ -3004,7 +3026,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="7" t="s">
         <v>37</v>
       </c>
@@ -3013,7 +3035,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="7" t="s">
         <v>38</v>
       </c>
@@ -3022,7 +3044,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="7" t="s">
         <v>39</v>
       </c>
@@ -3031,7 +3053,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="7" t="s">
         <v>40</v>
       </c>
@@ -3040,7 +3062,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="7" t="s">
         <v>41</v>
       </c>
@@ -3049,7 +3071,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="7" t="s">
         <v>42</v>
       </c>
@@ -3058,7 +3080,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="7" t="s">
         <v>43</v>
       </c>
@@ -3067,7 +3089,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="7" t="s">
         <v>44</v>
       </c>
@@ -3076,7 +3098,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="16"/>
       <c r="B38" s="7" t="s">
         <v>45</v>
       </c>
@@ -3085,7 +3107,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="16"/>
       <c r="B39" s="7" t="s">
         <v>46</v>
       </c>
@@ -3094,7 +3116,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="16"/>
       <c r="B40" s="7" t="s">
         <v>47</v>
       </c>
@@ -3103,7 +3125,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="16"/>
       <c r="B41" s="7" t="s">
         <v>48</v>
       </c>
@@ -3112,7 +3134,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="7" t="s">
         <v>49</v>
       </c>
@@ -3121,7 +3143,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="7" t="s">
         <v>50</v>
       </c>
@@ -3130,7 +3152,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="7" t="s">
         <v>51</v>
       </c>
@@ -3139,7 +3161,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
+      <c r="A45" s="16"/>
       <c r="B45" s="7" t="s">
         <v>52</v>
       </c>
@@ -3148,7 +3170,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="7" t="s">
         <v>53</v>
       </c>
@@ -3157,7 +3179,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="16"/>
       <c r="B47" s="7" t="s">
         <v>54</v>
       </c>
@@ -3166,7 +3188,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="A48" s="16"/>
       <c r="B48" s="7" t="s">
         <v>55</v>
       </c>
@@ -3175,7 +3197,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="16"/>
       <c r="B49" s="7" t="s">
         <v>56</v>
       </c>
@@ -3184,7 +3206,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="7" t="s">
         <v>57</v>
       </c>
@@ -3193,7 +3215,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="7" t="s">
         <v>58</v>
       </c>
@@ -3202,7 +3224,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="7" t="s">
         <v>59</v>
       </c>
@@ -3211,7 +3233,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="7" t="s">
         <v>60</v>
       </c>
@@ -3220,7 +3242,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="7" t="s">
         <v>61</v>
       </c>
@@ -3229,7 +3251,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="7" t="s">
         <v>62</v>
       </c>
@@ -3238,7 +3260,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
+      <c r="A56" s="16"/>
       <c r="B56" s="7" t="s">
         <v>63</v>
       </c>
@@ -3247,7 +3269,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="7" t="s">
         <v>64</v>
       </c>
@@ -3256,7 +3278,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
+      <c r="A58" s="16"/>
       <c r="B58" s="7" t="s">
         <v>65</v>
       </c>
@@ -3265,7 +3287,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="16"/>
       <c r="B59" s="7" t="s">
         <v>66</v>
       </c>
@@ -3274,7 +3296,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="16"/>
       <c r="B60" s="7" t="s">
         <v>67</v>
       </c>
@@ -3283,7 +3305,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
+      <c r="A61" s="16"/>
       <c r="B61" s="7" t="s">
         <v>68</v>
       </c>
@@ -3292,7 +3314,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="16"/>
       <c r="B62" s="7" t="s">
         <v>69</v>
       </c>
@@ -3301,7 +3323,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+      <c r="A63" s="16"/>
       <c r="B63" s="7" t="s">
         <v>70</v>
       </c>
@@ -3310,7 +3332,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="16"/>
       <c r="B64" s="7" t="s">
         <v>71</v>
       </c>
@@ -3319,7 +3341,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
+      <c r="A65" s="16"/>
       <c r="B65" s="7" t="s">
         <v>72</v>
       </c>
@@ -3328,7 +3350,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
+      <c r="A66" s="16"/>
       <c r="B66" s="7" t="s">
         <v>73</v>
       </c>
@@ -3337,7 +3359,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
+      <c r="A67" s="16"/>
       <c r="B67" s="7" t="s">
         <v>74</v>
       </c>
@@ -3346,7 +3368,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="16"/>
       <c r="B68" s="7" t="s">
         <v>75</v>
       </c>
@@ -3355,7 +3377,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
+      <c r="A69" s="16"/>
       <c r="B69" s="7" t="s">
         <v>76</v>
       </c>
@@ -3364,7 +3386,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="7" t="s">
         <v>77</v>
       </c>
@@ -3373,7 +3395,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
+      <c r="A71" s="16"/>
       <c r="B71" s="7" t="s">
         <v>78</v>
       </c>
@@ -3382,7 +3404,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
+      <c r="A72" s="16"/>
       <c r="B72" s="7" t="s">
         <v>79</v>
       </c>
@@ -3391,7 +3413,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
+      <c r="A73" s="16"/>
       <c r="B73" s="7" t="s">
         <v>80</v>
       </c>
@@ -3400,7 +3422,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
+      <c r="A74" s="16"/>
       <c r="B74" s="7" t="s">
         <v>81</v>
       </c>
@@ -3409,7 +3431,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="16"/>
       <c r="B75" s="7" t="s">
         <v>82</v>
       </c>
@@ -3418,7 +3440,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
+      <c r="A76" s="16"/>
       <c r="B76" s="7" t="s">
         <v>83</v>
       </c>
@@ -3427,7 +3449,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
+      <c r="A77" s="16"/>
       <c r="B77" s="7" t="s">
         <v>84</v>
       </c>
@@ -3436,7 +3458,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="14"/>
+      <c r="A78" s="16"/>
       <c r="B78" s="7" t="s">
         <v>85</v>
       </c>
@@ -3445,7 +3467,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
+      <c r="A79" s="16"/>
       <c r="B79" s="7" t="s">
         <v>86</v>
       </c>
@@ -3454,7 +3476,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
+      <c r="A80" s="16"/>
       <c r="B80" s="7" t="s">
         <v>87</v>
       </c>
@@ -3463,7 +3485,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
+      <c r="A81" s="16"/>
       <c r="B81" s="7" t="s">
         <v>88</v>
       </c>
@@ -3472,7 +3494,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
+      <c r="A82" s="16"/>
       <c r="B82" s="7" t="s">
         <v>89</v>
       </c>
@@ -3481,7 +3503,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
+      <c r="A83" s="16"/>
       <c r="B83" s="7" t="s">
         <v>90</v>
       </c>
@@ -3490,7 +3512,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
+      <c r="A84" s="16"/>
       <c r="B84" s="7" t="s">
         <v>91</v>
       </c>
@@ -3499,7 +3521,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
+      <c r="A85" s="16"/>
       <c r="B85" s="7" t="s">
         <v>92</v>
       </c>
@@ -3508,7 +3530,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
+      <c r="A86" s="16"/>
       <c r="B86" s="7" t="s">
         <v>93</v>
       </c>
@@ -3545,16 +3567,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>139</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3571,7 +3593,7 @@
         <v>114</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>